<commit_message>
Elements - Web Tables
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -41,6 +41,183 @@
   </si>
   <si>
     <t>Elements</t>
+  </si>
+  <si>
+    <t>Text Box</t>
+  </si>
+  <si>
+    <t>textBoxNav</t>
+  </si>
+  <si>
+    <t>//*[@id="item-0"]</t>
+  </si>
+  <si>
+    <t>fullName</t>
+  </si>
+  <si>
+    <t>//*[@id="userName"]</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>//*[@id="userEmail"]</t>
+  </si>
+  <si>
+    <t>currentAddress</t>
+  </si>
+  <si>
+    <t>//*[@id="currentAddress"]</t>
+  </si>
+  <si>
+    <t>permanentAddress</t>
+  </si>
+  <si>
+    <t>//*[@id="permanentAddress"]</t>
+  </si>
+  <si>
+    <t>submitButton</t>
+  </si>
+  <si>
+    <t>//*[@id="submit"]</t>
+  </si>
+  <si>
+    <t>Check Box</t>
+  </si>
+  <si>
+    <t>selectedCheckboxOutput</t>
+  </si>
+  <si>
+    <t>//*[@id="result"]/span[1]</t>
+  </si>
+  <si>
+    <t>checkBoxNav</t>
+  </si>
+  <si>
+    <t>//*[@id="item-1"]</t>
+  </si>
+  <si>
+    <t>expandAllButton</t>
+  </si>
+  <si>
+    <t>//*[@id="tree-node"]/div/button[1]</t>
+  </si>
+  <si>
+    <t>homeCheckbox</t>
+  </si>
+  <si>
+    <t>//*[@id="tree-node"]/ol/li/span/label/span[1]</t>
+  </si>
+  <si>
+    <t>radioButton</t>
+  </si>
+  <si>
+    <t>radioButtonNav</t>
+  </si>
+  <si>
+    <t>//*[@id="item-2"]</t>
+  </si>
+  <si>
+    <t>yesRadio</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div/div/div/div[2]/div[2]/div[2]/label</t>
+  </si>
+  <si>
+    <t>selectedRadioOutput</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div/div/div/div[2]/div[2]/p</t>
+  </si>
+  <si>
+    <t>WebTable</t>
+  </si>
+  <si>
+    <t>scrollWebTables</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div/div/div/div[2]/h1</t>
+  </si>
+  <si>
+    <t>webTablesNav</t>
+  </si>
+  <si>
+    <t>//*[@id="item-3"]</t>
+  </si>
+  <si>
+    <t>addButton</t>
+  </si>
+  <si>
+    <t>//*[@id="addNewRecordButton"]</t>
+  </si>
+  <si>
+    <t>formScroll</t>
+  </si>
+  <si>
+    <t>//*[@id="registration-form-modal"]</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>//*[@id="firstName"]</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>//*[@id="lastName"]</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>//*[@id="age"]</t>
+  </si>
+  <si>
+    <t>salary</t>
+  </si>
+  <si>
+    <t>//*[@id="salary"]</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>//*[@id="department"]</t>
+  </si>
+  <si>
+    <t>webTableSubmit</t>
+  </si>
+  <si>
+    <t>tableOutput</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div/div/div/div[2]/div[2]/div[3]/div[1]/div[2]/div[4]/div/div[1]</t>
+  </si>
+  <si>
+    <t>addedUserEdit</t>
+  </si>
+  <si>
+    <t>//*[@id="edit-record-4"]</t>
+  </si>
+  <si>
+    <t>addedUserDelete</t>
+  </si>
+  <si>
+    <t>//*[@id="delete-record-4"]</t>
+  </si>
+  <si>
+    <t>editedTableOutput</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div/div/div/div[2]/div[2]/div[3]/div[1]/div[2]/div[4]/div/div[5]</t>
+  </si>
+  <si>
+    <t>webTableUserDlt</t>
+  </si>
+  <si>
+    <t>//*[@id="delete-record-4"]/svg/path</t>
   </si>
 </sst>
 </file>
@@ -305,8 +482,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A21">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
@@ -359,101 +536,347 @@
       <c r="C5" s="3"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="C7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="C8" s="1"/>
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="C9" s="1"/>
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="C10" s="1"/>
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="C11" s="1"/>
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="C12" s="1"/>
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="C14" s="1"/>
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="C15" s="1"/>
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="C16" s="1"/>
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="C17" s="1"/>
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="C19" s="1"/>
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="C20" s="1"/>
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="4"/>
-      <c r="C21" s="1"/>
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="4"/>
+      <c r="A22" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="4"/>
-      <c r="C23" s="1"/>
+      <c r="A23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="4"/>
-      <c r="C24" s="1"/>
+      <c r="A24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="4"/>
-      <c r="C25" s="1"/>
+      <c r="A25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="C26" s="1"/>
+      <c r="A26" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="C27" s="1"/>
+      <c r="A27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="C28" s="1"/>
+      <c r="A28" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="C29" s="1"/>
+      <c r="A29" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="C30" s="1"/>
+      <c r="A30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="C31" s="1"/>
+      <c r="A31" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="C32" s="1"/>
+      <c r="A32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
+      <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" ht="14.25" customHeight="1">
+      <c r="A34" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" ht="14.25" customHeight="1">
+      <c r="A36" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" ht="14.25" customHeight="1">
+      <c r="A37" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" ht="14.25" customHeight="1">
+      <c r="A38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="39" ht="14.25" customHeight="1"/>
     <row r="40" ht="14.25" customHeight="1"/>
     <row r="41" ht="14.25" customHeight="1"/>
@@ -1405,6 +1828,10 @@
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
     <row r="989" ht="14.25" customHeight="1"/>
+    <row r="990" ht="14.25" customHeight="1"/>
+    <row r="991" ht="14.25" customHeight="1"/>
+    <row r="992" ht="14.25" customHeight="1"/>
+    <row r="993" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:C2"/>

</xml_diff>

<commit_message>
Elements - broken links
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -326,6 +326,24 @@
   </si>
   <si>
     <t>//*[@id="linkWrapper"]/h5[2]/strong</t>
+  </si>
+  <si>
+    <t>brokenLinks</t>
+  </si>
+  <si>
+    <t>brokenLinksNav</t>
+  </si>
+  <si>
+    <t>//*[@id="item-6"]</t>
+  </si>
+  <si>
+    <t>brokenLink</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div/div/div/div[2]/div[2]/a[2]</t>
+  </si>
+  <si>
+    <t>brokenLinkScroll</t>
   </si>
 </sst>
 </file>
@@ -590,8 +608,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A43">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A46">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
@@ -1182,10 +1200,44 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
+    <row r="58" ht="14.25" customHeight="1">
+      <c r="A58" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="59" ht="14.25" customHeight="1">
+      <c r="A59" t="s">
+        <v>104</v>
+      </c>
+      <c r="B59" t="s">
+        <v>105</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" ht="14.25" customHeight="1">
+      <c r="A60" t="s">
+        <v>106</v>
+      </c>
+      <c r="B60" t="s">
+        <v>107</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" ht="14.25" customHeight="1">
+      <c r="A61" t="s">
+        <v>108</v>
+      </c>
+      <c r="B61" t="s">
+        <v>71</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="62" ht="14.25" customHeight="1"/>
     <row r="63" ht="14.25" customHeight="1"/>
     <row r="64" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Elements - Upload and Download
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -344,6 +344,36 @@
   </si>
   <si>
     <t>brokenLinkScroll</t>
+  </si>
+  <si>
+    <t>uploadDownload</t>
+  </si>
+  <si>
+    <t>uploadDownloadNav</t>
+  </si>
+  <si>
+    <t>//*[@id="item-7"]</t>
+  </si>
+  <si>
+    <t>uploadDownloadScroll</t>
+  </si>
+  <si>
+    <t>imgDownloadBtn</t>
+  </si>
+  <si>
+    <t>//*[@id="downloadButton"]</t>
+  </si>
+  <si>
+    <t>uploadFileInput</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div/div/div/div[2]/div[2]/div[2]/form/div</t>
+  </si>
+  <si>
+    <t>uploadedFileName</t>
+  </si>
+  <si>
+    <t>//*[@id="uploadedFilePath"]</t>
   </si>
 </sst>
 </file>
@@ -608,8 +638,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A46">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A55">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
@@ -1238,12 +1268,66 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
+    <row r="62" ht="14.25" customHeight="1">
+      <c r="A62" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="63" ht="14.25" customHeight="1">
+      <c r="A63" t="s">
+        <v>110</v>
+      </c>
+      <c r="B63" t="s">
+        <v>111</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" ht="14.25" customHeight="1">
+      <c r="A64" t="s">
+        <v>112</v>
+      </c>
+      <c r="B64" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" ht="14.25" customHeight="1">
+      <c r="A65" t="s">
+        <v>113</v>
+      </c>
+      <c r="B65" t="s">
+        <v>114</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" ht="14.25" customHeight="1">
+      <c r="A66" t="s">
+        <v>115</v>
+      </c>
+      <c r="B66" t="s">
+        <v>116</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" ht="14.25" customHeight="1">
+      <c r="A67" t="s">
+        <v>117</v>
+      </c>
+      <c r="B67" t="s">
+        <v>118</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="68" ht="14.25" customHeight="1"/>
     <row r="69" ht="14.25" customHeight="1"/>
     <row r="70" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Elements - Dynamic Properties
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -374,6 +374,36 @@
   </si>
   <si>
     <t>//*[@id="uploadedFilePath"]</t>
+  </si>
+  <si>
+    <t>dynamicProperties</t>
+  </si>
+  <si>
+    <t>dynamicPropertiesNav</t>
+  </si>
+  <si>
+    <t>//*[@id="item-8"]</t>
+  </si>
+  <si>
+    <t>dynamicPropertiesScroll</t>
+  </si>
+  <si>
+    <t>enableBtn</t>
+  </si>
+  <si>
+    <t>//*[@id="enableAfter"]</t>
+  </si>
+  <si>
+    <t>ColorBtn</t>
+  </si>
+  <si>
+    <t>//*[@id="colorChange"]</t>
+  </si>
+  <si>
+    <t>Visiblbtn</t>
+  </si>
+  <si>
+    <t>//*[@id="visibleAfter"]</t>
   </si>
 </sst>
 </file>
@@ -638,8 +668,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A55">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A61">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
@@ -1328,12 +1358,66 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
+    <row r="68" ht="14.25" customHeight="1">
+      <c r="A68" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="69" ht="14.25" customHeight="1">
+      <c r="A69" t="s">
+        <v>120</v>
+      </c>
+      <c r="B69" t="s">
+        <v>121</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" ht="14.25" customHeight="1">
+      <c r="A70" t="s">
+        <v>122</v>
+      </c>
+      <c r="B70" t="s">
+        <v>71</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" ht="14.25" customHeight="1">
+      <c r="A71" t="s">
+        <v>123</v>
+      </c>
+      <c r="B71" t="s">
+        <v>124</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" ht="14.25" customHeight="1">
+      <c r="A72" t="s">
+        <v>125</v>
+      </c>
+      <c r="B72" t="s">
+        <v>126</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" ht="14.25" customHeight="1">
+      <c r="A73" t="s">
+        <v>127</v>
+      </c>
+      <c r="B73" t="s">
+        <v>128</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="74" ht="14.25" customHeight="1"/>
     <row r="75" ht="14.25" customHeight="1"/>
     <row r="76" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Forms - Practice Form
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -40,6 +40,12 @@
     <t>By.xpath</t>
   </si>
   <si>
+    <t>forms</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div/div/div[2]/div/div[2]/div</t>
+  </si>
+  <si>
     <t>Elements</t>
   </si>
   <si>
@@ -404,6 +410,81 @@
   </si>
   <si>
     <t>//*[@id="visibleAfter"]</t>
+  </si>
+  <si>
+    <t>Forms</t>
+  </si>
+  <si>
+    <t>practiceForm</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div/div/div/div[1]/div/div/div[2]/div</t>
+  </si>
+  <si>
+    <t>formsFirstName</t>
+  </si>
+  <si>
+    <t>formsLastName</t>
+  </si>
+  <si>
+    <t>formsEmail</t>
+  </si>
+  <si>
+    <t>formsGender</t>
+  </si>
+  <si>
+    <t>//*[@id="genterWrapper"]/div[2]/div[2]/label</t>
+  </si>
+  <si>
+    <t>formsMobile</t>
+  </si>
+  <si>
+    <t>//*[@id="userNumber"]</t>
+  </si>
+  <si>
+    <t>formsDateOfBirth</t>
+  </si>
+  <si>
+    <t>//*[@id="dateOfBirthInput"]</t>
+  </si>
+  <si>
+    <t>formsSubjects</t>
+  </si>
+  <si>
+    <t>//*[@id="subjectsContainer"]/div/div[1]</t>
+  </si>
+  <si>
+    <t>formsHobbiesReading</t>
+  </si>
+  <si>
+    <t>//*[@id="hobbiesWrapper"]/div[2]/div[2]/label</t>
+  </si>
+  <si>
+    <t>formsHobbiesMusic</t>
+  </si>
+  <si>
+    <t>//*[@id="hobbiesWrapper"]/div[2]/div[3]/label</t>
+  </si>
+  <si>
+    <t>formsUploadPicture</t>
+  </si>
+  <si>
+    <t>//*[@id="uploadPicture"]</t>
+  </si>
+  <si>
+    <t>formsAddress</t>
+  </si>
+  <si>
+    <t>formsSubmitButton</t>
+  </si>
+  <si>
+    <t>practiceFormScroll</t>
+  </si>
+  <si>
+    <t>formsScroll</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div/div/div/div[1]/div/div/div[2]/span/div</t>
   </si>
 </sst>
 </file>
@@ -668,8 +749,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A61">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A73">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
@@ -710,28 +791,34 @@
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" ht="22.5" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
@@ -739,10 +826,10 @@
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
@@ -750,10 +837,10 @@
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>6</v>
@@ -761,10 +848,10 @@
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>6</v>
@@ -772,10 +859,10 @@
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>6</v>
@@ -783,10 +870,10 @@
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>6</v>
@@ -794,16 +881,16 @@
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>6</v>
@@ -811,10 +898,10 @@
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>6</v>
@@ -822,10 +909,10 @@
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>6</v>
@@ -833,10 +920,10 @@
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>6</v>
@@ -844,16 +931,16 @@
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>6</v>
@@ -861,10 +948,10 @@
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>6</v>
@@ -872,10 +959,10 @@
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>6</v>
@@ -883,16 +970,16 @@
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>6</v>
@@ -900,10 +987,10 @@
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>6</v>
@@ -911,10 +998,10 @@
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>6</v>
@@ -922,10 +1009,10 @@
     </row>
     <row r="26" ht="14.25" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>6</v>
@@ -933,10 +1020,10 @@
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>6</v>
@@ -944,10 +1031,10 @@
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>6</v>
@@ -955,10 +1042,10 @@
     </row>
     <row r="29" ht="14.25" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>6</v>
@@ -966,10 +1053,10 @@
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>6</v>
@@ -977,10 +1064,10 @@
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>6</v>
@@ -988,10 +1075,10 @@
     </row>
     <row r="32" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B32" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>6</v>
@@ -999,10 +1086,10 @@
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>6</v>
@@ -1010,10 +1097,10 @@
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>6</v>
@@ -1021,10 +1108,10 @@
     </row>
     <row r="35" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>6</v>
@@ -1032,10 +1119,10 @@
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>6</v>
@@ -1043,10 +1130,10 @@
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B37" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>6</v>
@@ -1054,10 +1141,10 @@
     </row>
     <row r="38" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B38" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>6</v>
@@ -1065,15 +1152,15 @@
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B40" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>6</v>
@@ -1081,10 +1168,10 @@
     </row>
     <row r="41" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B41" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>6</v>
@@ -1092,10 +1179,10 @@
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B42" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>6</v>
@@ -1103,10 +1190,10 @@
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B43" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>6</v>
@@ -1114,10 +1201,10 @@
     </row>
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B44" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>6</v>
@@ -1125,10 +1212,10 @@
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B45" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>6</v>
@@ -1136,10 +1223,10 @@
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B46" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>6</v>
@@ -1147,10 +1234,10 @@
     </row>
     <row r="47" ht="14.25" customHeight="1">
       <c r="A47" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B47" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>6</v>
@@ -1158,15 +1245,15 @@
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B49" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>6</v>
@@ -1174,10 +1261,10 @@
     </row>
     <row r="50" ht="14.25" customHeight="1">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B50" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>6</v>
@@ -1185,10 +1272,10 @@
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B51" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>6</v>
@@ -1196,10 +1283,10 @@
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B52" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>6</v>
@@ -1207,10 +1294,10 @@
     </row>
     <row r="53" ht="14.25" customHeight="1">
       <c r="A53" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B53" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>6</v>
@@ -1218,10 +1305,10 @@
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B54" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>6</v>
@@ -1229,10 +1316,10 @@
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B55" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>6</v>
@@ -1240,10 +1327,10 @@
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B56" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>6</v>
@@ -1251,10 +1338,10 @@
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B57" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>6</v>
@@ -1262,15 +1349,15 @@
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
       <c r="A59" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B59" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>6</v>
@@ -1278,10 +1365,10 @@
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B60" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>6</v>
@@ -1289,10 +1376,10 @@
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B61" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>6</v>
@@ -1300,15 +1387,15 @@
     </row>
     <row r="62" ht="14.25" customHeight="1">
       <c r="A62" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B63" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>6</v>
@@ -1316,10 +1403,10 @@
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B64" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>6</v>
@@ -1327,10 +1414,10 @@
     </row>
     <row r="65" ht="14.25" customHeight="1">
       <c r="A65" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B65" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>6</v>
@@ -1338,10 +1425,10 @@
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B66" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>6</v>
@@ -1349,10 +1436,10 @@
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B67" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>6</v>
@@ -1360,15 +1447,15 @@
     </row>
     <row r="68" ht="14.25" customHeight="1">
       <c r="A68" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B69" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>6</v>
@@ -1376,10 +1463,10 @@
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B70" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>6</v>
@@ -1387,10 +1474,10 @@
     </row>
     <row r="71" ht="14.25" customHeight="1">
       <c r="A71" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B71" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>6</v>
@@ -1398,10 +1485,10 @@
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B72" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>6</v>
@@ -1409,32 +1496,188 @@
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B73" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
+    <row r="75" ht="22.5" customHeight="1">
+      <c r="A75" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+    </row>
+    <row r="76" ht="14.25" customHeight="1">
+      <c r="A76" t="s">
+        <v>132</v>
+      </c>
+      <c r="B76" t="s">
+        <v>133</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" ht="14.25" customHeight="1">
+      <c r="A77" t="s">
+        <v>134</v>
+      </c>
+      <c r="B77" t="s">
+        <v>49</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" ht="14.25" customHeight="1">
+      <c r="A78" t="s">
+        <v>135</v>
+      </c>
+      <c r="B78" t="s">
+        <v>51</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" ht="14.25" customHeight="1">
+      <c r="A79" t="s">
+        <v>136</v>
+      </c>
+      <c r="B79" t="s">
+        <v>16</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" ht="14.25" customHeight="1">
+      <c r="A80" t="s">
+        <v>137</v>
+      </c>
+      <c r="B80" t="s">
+        <v>138</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" ht="14.25" customHeight="1">
+      <c r="A81" t="s">
+        <v>139</v>
+      </c>
+      <c r="B81" t="s">
+        <v>140</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" ht="14.25" customHeight="1">
+      <c r="A82" t="s">
+        <v>141</v>
+      </c>
+      <c r="B82" t="s">
+        <v>142</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" ht="14.25" customHeight="1">
+      <c r="A83" t="s">
+        <v>143</v>
+      </c>
+      <c r="B83" t="s">
+        <v>144</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" ht="14.25" customHeight="1">
+      <c r="A84" t="s">
+        <v>145</v>
+      </c>
+      <c r="B84" t="s">
+        <v>146</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" ht="14.25" customHeight="1">
+      <c r="A85" t="s">
+        <v>147</v>
+      </c>
+      <c r="B85" t="s">
+        <v>148</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" ht="14.25" customHeight="1">
+      <c r="A86" t="s">
+        <v>149</v>
+      </c>
+      <c r="B86" t="s">
+        <v>150</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" ht="14.25" customHeight="1">
+      <c r="A87" t="s">
+        <v>151</v>
+      </c>
+      <c r="B87" t="s">
+        <v>18</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" ht="14.25" customHeight="1">
+      <c r="A88" t="s">
+        <v>152</v>
+      </c>
+      <c r="B88" t="s">
+        <v>22</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" ht="14.25" customHeight="1">
+      <c r="A89" t="s">
+        <v>153</v>
+      </c>
+      <c r="B89" t="s">
+        <v>73</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" ht="14.25" customHeight="1">
+      <c r="A90" t="s">
+        <v>154</v>
+      </c>
+      <c r="B90" t="s">
+        <v>155</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="91" ht="14.25" customHeight="1"/>
     <row r="92" ht="14.25" customHeight="1"/>
     <row r="93" ht="14.25" customHeight="1"/>
@@ -2338,10 +2581,12 @@
     <row r="991" ht="14.25" customHeight="1"/>
     <row r="992" ht="14.25" customHeight="1"/>
     <row r="993" ht="14.25" customHeight="1"/>
+    <row r="994" ht="14.25" customHeight="1"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A75:C75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Alerts, Frame & Windows - BrowserWindows
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -40,6 +40,12 @@
     <t>By.xpath</t>
   </si>
   <si>
+    <t>AlertsFramesWindows</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div/div/div[2]/div/div[3]/div</t>
+  </si>
+  <si>
     <t>forms</t>
   </si>
   <si>
@@ -485,6 +491,39 @@
   </si>
   <si>
     <t>//*[@id="app"]/div/div/div/div[1]/div/div/div[2]/span/div</t>
+  </si>
+  <si>
+    <t>Alerts, Frame &amp; Windows</t>
+  </si>
+  <si>
+    <t>firstScrollAlert</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div/div/div/div[1]/div/div/div[3]/span</t>
+  </si>
+  <si>
+    <t>browserWindowsNav</t>
+  </si>
+  <si>
+    <t>//div[@class='element-list collapse show']//li[@id='item-0']</t>
+  </si>
+  <si>
+    <t>newTabButton</t>
+  </si>
+  <si>
+    <t>//*[@id="tabButton"]</t>
+  </si>
+  <si>
+    <t>newWindow</t>
+  </si>
+  <si>
+    <t>//*[@id="windowButton"]</t>
+  </si>
+  <si>
+    <t>newWindowMessage</t>
+  </si>
+  <si>
+    <t>//*[@id="messageWindowButton"]</t>
   </si>
 </sst>
 </file>
@@ -749,8 +788,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A73">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A85">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
@@ -791,44 +830,44 @@
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" ht="22.5" customHeight="1">
-      <c r="A5" s="2" t="s">
+    <row r="5" ht="14.25" customHeight="1">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" ht="22.5" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -883,18 +922,18 @@
       <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="C14" s="1"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" t="s">
@@ -933,18 +972,18 @@
       <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="C19" s="1"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" t="s">
@@ -969,21 +1008,21 @@
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="4" t="s">
+      <c r="A22" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="1"/>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="C23" s="1"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="4" t="s">
@@ -1042,21 +1081,21 @@
     </row>
     <row r="29" ht="14.25" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" t="s">
-        <v>52</v>
+      <c r="A30" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>6</v>
@@ -1089,7 +1128,7 @@
         <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>6</v>
@@ -1097,10 +1136,10 @@
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B34" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>6</v>
@@ -1154,16 +1193,16 @@
       <c r="A39" t="s">
         <v>69</v>
       </c>
+      <c r="B39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>70</v>
-      </c>
-      <c r="B40" t="s">
         <v>71</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -1247,16 +1286,16 @@
       <c r="A48" t="s">
         <v>86</v>
       </c>
+      <c r="B48" t="s">
+        <v>87</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" t="s">
-        <v>87</v>
-      </c>
-      <c r="B49" t="s">
         <v>88</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -1351,16 +1390,16 @@
       <c r="A58" t="s">
         <v>105</v>
       </c>
+      <c r="B58" t="s">
+        <v>106</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
       <c r="A59" t="s">
-        <v>106</v>
-      </c>
-      <c r="B59" t="s">
         <v>107</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="60" ht="14.25" customHeight="1">
@@ -1379,7 +1418,7 @@
         <v>110</v>
       </c>
       <c r="B61" t="s">
-        <v>73</v>
+        <v>111</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>6</v>
@@ -1387,18 +1426,18 @@
     </row>
     <row r="62" ht="14.25" customHeight="1">
       <c r="A62" t="s">
-        <v>111</v>
+        <v>112</v>
+      </c>
+      <c r="B62" t="s">
+        <v>75</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" t="s">
-        <v>112</v>
-      </c>
-      <c r="B63" t="s">
         <v>113</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
@@ -1406,7 +1445,7 @@
         <v>114</v>
       </c>
       <c r="B64" t="s">
-        <v>73</v>
+        <v>115</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>6</v>
@@ -1414,10 +1453,10 @@
     </row>
     <row r="65" ht="14.25" customHeight="1">
       <c r="A65" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B65" t="s">
-        <v>116</v>
+        <v>75</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>6</v>
@@ -1449,16 +1488,16 @@
       <c r="A68" t="s">
         <v>121</v>
       </c>
+      <c r="B68" t="s">
+        <v>122</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" t="s">
-        <v>122</v>
-      </c>
-      <c r="B69" t="s">
         <v>123</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
@@ -1466,7 +1505,7 @@
         <v>124</v>
       </c>
       <c r="B70" t="s">
-        <v>73</v>
+        <v>125</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>6</v>
@@ -1474,10 +1513,10 @@
     </row>
     <row r="71" ht="14.25" customHeight="1">
       <c r="A71" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B71" t="s">
-        <v>126</v>
+        <v>75</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>6</v>
@@ -1505,31 +1544,31 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="22.5" customHeight="1">
-      <c r="A75" s="2" t="s">
+    <row r="74" ht="14.25" customHeight="1">
+      <c r="A74" t="s">
         <v>131</v>
       </c>
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-    </row>
-    <row r="76" ht="14.25" customHeight="1">
-      <c r="A76" t="s">
+      <c r="B74" t="s">
         <v>132</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C74" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" ht="14.25" customHeight="1"/>
+    <row r="76" ht="22.5" customHeight="1">
+      <c r="A76" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
     </row>
     <row r="77" ht="14.25" customHeight="1">
       <c r="A77" t="s">
         <v>134</v>
       </c>
       <c r="B77" t="s">
-        <v>49</v>
+        <v>135</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>6</v>
@@ -1537,7 +1576,7 @@
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B78" t="s">
         <v>51</v>
@@ -1548,10 +1587,10 @@
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B79" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>6</v>
@@ -1559,10 +1598,10 @@
     </row>
     <row r="80" ht="14.25" customHeight="1">
       <c r="A80" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B80" t="s">
-        <v>138</v>
+        <v>18</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>6</v>
@@ -1639,7 +1678,7 @@
         <v>151</v>
       </c>
       <c r="B87" t="s">
-        <v>18</v>
+        <v>152</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>6</v>
@@ -1647,10 +1686,10 @@
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B88" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>6</v>
@@ -1658,10 +1697,10 @@
     </row>
     <row r="89" ht="14.25" customHeight="1">
       <c r="A89" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B89" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>6</v>
@@ -1669,22 +1708,88 @@
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B90" t="s">
-        <v>155</v>
+        <v>75</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
+    <row r="91" ht="14.25" customHeight="1">
+      <c r="A91" t="s">
+        <v>156</v>
+      </c>
+      <c r="B91" t="s">
+        <v>157</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" ht="22.5" customHeight="1">
+      <c r="A92" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+    </row>
+    <row r="93" ht="22.5" customHeight="1">
+      <c r="A93" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" ht="14.25" customHeight="1">
+      <c r="A94" t="s">
+        <v>161</v>
+      </c>
+      <c r="B94" t="s">
+        <v>162</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" ht="14.25" customHeight="1">
+      <c r="A95" t="s">
+        <v>163</v>
+      </c>
+      <c r="B95" t="s">
+        <v>164</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" ht="14.25" customHeight="1">
+      <c r="A96" t="s">
+        <v>165</v>
+      </c>
+      <c r="B96" t="s">
+        <v>166</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" ht="14.25" customHeight="1">
+      <c r="A97" t="s">
+        <v>167</v>
+      </c>
+      <c r="B97" t="s">
+        <v>168</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="98" ht="14.25" customHeight="1"/>
     <row r="99" ht="14.25" customHeight="1"/>
     <row r="100" ht="14.25" customHeight="1"/>
@@ -2582,11 +2687,13 @@
     <row r="992" ht="14.25" customHeight="1"/>
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
+    <row r="995" ht="14.25" customHeight="1"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A75:C75"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A76:C76"/>
+    <mergeCell ref="A92:C92"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Alerts, Frame & Windows - Alerts
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -524,6 +524,45 @@
   </si>
   <si>
     <t>//*[@id="messageWindowButton"]</t>
+  </si>
+  <si>
+    <t>Alerts</t>
+  </si>
+  <si>
+    <t>alertsNav</t>
+  </si>
+  <si>
+    <t>//div[@class='element-list collapse show']//li[@id='item-1']</t>
+  </si>
+  <si>
+    <t>alertsScroll</t>
+  </si>
+  <si>
+    <t>//h1[normalize-space()='Alerts']</t>
+  </si>
+  <si>
+    <t>alertBtn</t>
+  </si>
+  <si>
+    <t>//button[@id='alertButton']</t>
+  </si>
+  <si>
+    <t>fiveMinBtn</t>
+  </si>
+  <si>
+    <t>//button[@id='timerAlertButton']</t>
+  </si>
+  <si>
+    <t>confirmBoxBtn</t>
+  </si>
+  <si>
+    <t>//button[@id='confirmButton']</t>
+  </si>
+  <si>
+    <t>promptBtn</t>
+  </si>
+  <si>
+    <t>//button[@id='promtButton']</t>
   </si>
 </sst>
 </file>
@@ -789,7 +828,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A85">
-      <selection activeCell="B100" sqref="B100"/>
+      <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
@@ -1790,13 +1829,77 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
-    <row r="101" ht="14.25" customHeight="1"/>
-    <row r="102" ht="14.25" customHeight="1"/>
-    <row r="103" ht="14.25" customHeight="1"/>
-    <row r="104" ht="14.25" customHeight="1"/>
+    <row r="98" ht="14.25" customHeight="1">
+      <c r="A98" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="99" ht="14.25" customHeight="1">
+      <c r="A99" t="s">
+        <v>170</v>
+      </c>
+      <c r="B99" t="s">
+        <v>171</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" ht="14.25" customHeight="1">
+      <c r="A100" t="s">
+        <v>172</v>
+      </c>
+      <c r="B100" t="s">
+        <v>173</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" ht="14.25" customHeight="1">
+      <c r="A101" t="s">
+        <v>174</v>
+      </c>
+      <c r="B101" t="s">
+        <v>175</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" ht="14.25" customHeight="1">
+      <c r="A102" t="s">
+        <v>176</v>
+      </c>
+      <c r="B102" t="s">
+        <v>177</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" ht="14.25" customHeight="1">
+      <c r="A103" t="s">
+        <v>178</v>
+      </c>
+      <c r="B103" t="s">
+        <v>179</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" ht="14.25" customHeight="1">
+      <c r="A104" t="s">
+        <v>180</v>
+      </c>
+      <c r="B104" t="s">
+        <v>181</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="105" ht="14.25" customHeight="1"/>
     <row r="106" ht="14.25" customHeight="1"/>
     <row r="107" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Alerts, Frame & Windows - Frames
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -563,6 +563,36 @@
   </si>
   <si>
     <t>//button[@id='promtButton']</t>
+  </si>
+  <si>
+    <t>Frames</t>
+  </si>
+  <si>
+    <t>framesNav</t>
+  </si>
+  <si>
+    <t>//div[@class='element-list collapse show']//li[@id='item-2']</t>
+  </si>
+  <si>
+    <t>frame1</t>
+  </si>
+  <si>
+    <t>//*[@id="frame1"]</t>
+  </si>
+  <si>
+    <t>frame1Heading</t>
+  </si>
+  <si>
+    <t>//*[@id="sampleHeading"]</t>
+  </si>
+  <si>
+    <t>frame2</t>
+  </si>
+  <si>
+    <t>//*[@id="frame2"]</t>
+  </si>
+  <si>
+    <t>frame2Heading</t>
   </si>
 </sst>
 </file>
@@ -827,8 +857,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A85">
-      <selection activeCell="B104" sqref="B104"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A88">
+      <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
@@ -1900,12 +1930,66 @@
         <v>6</v>
       </c>
     </row>
-    <row r="105" ht="14.25" customHeight="1"/>
-    <row r="106" ht="14.25" customHeight="1"/>
-    <row r="107" ht="14.25" customHeight="1"/>
-    <row r="108" ht="14.25" customHeight="1"/>
-    <row r="109" ht="14.25" customHeight="1"/>
-    <row r="110" ht="14.25" customHeight="1"/>
+    <row r="105" ht="14.25" customHeight="1">
+      <c r="A105" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="106" ht="14.25" customHeight="1">
+      <c r="A106" t="s">
+        <v>183</v>
+      </c>
+      <c r="B106" t="s">
+        <v>184</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" ht="14.25" customHeight="1">
+      <c r="A107" t="s">
+        <v>185</v>
+      </c>
+      <c r="B107" t="s">
+        <v>186</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" ht="14.25" customHeight="1">
+      <c r="A108" t="s">
+        <v>187</v>
+      </c>
+      <c r="B108" t="s">
+        <v>188</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" ht="14.25" customHeight="1">
+      <c r="A109" t="s">
+        <v>189</v>
+      </c>
+      <c r="B109" t="s">
+        <v>190</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" ht="14.25" customHeight="1">
+      <c r="A110" t="s">
+        <v>191</v>
+      </c>
+      <c r="B110" t="s">
+        <v>188</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="111" ht="14.25" customHeight="1"/>
     <row r="112" ht="14.25" customHeight="1"/>
     <row r="113" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Widgets - Date picker
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -713,6 +713,51 @@
   </si>
   <si>
     <t>clickWidgtsToOpen</t>
+  </si>
+  <si>
+    <t>Auto Complete</t>
+  </si>
+  <si>
+    <t>autoCompleteNav</t>
+  </si>
+  <si>
+    <t>autoCompleteInput</t>
+  </si>
+  <si>
+    <t>//*[@id="autoCompleteMultipleContainer"]</t>
+  </si>
+  <si>
+    <t>suggestion1</t>
+  </si>
+  <si>
+    <t>//*[@id="react-select-8-option-0"]</t>
+  </si>
+  <si>
+    <t>//*[@id="autoCompleteMultipleContainer"]/div/div[1]/div[1]/div[1]</t>
+  </si>
+  <si>
+    <t>datePicker</t>
+  </si>
+  <si>
+    <t>datePickerNav</t>
+  </si>
+  <si>
+    <t>WidgetsScroll</t>
+  </si>
+  <si>
+    <t>//body/div[@id='app']/div[@class='body-height']/div[@class='container playgound-body']/div[@class='row']/div[1]/div[1]/div[1]/div[4]/span[1]/div[1]</t>
+  </si>
+  <si>
+    <t>datePickerInput</t>
+  </si>
+  <si>
+    <t>//*[@id="datePickerMonthYear"]/div</t>
+  </si>
+  <si>
+    <t>datePickerSelectedDate</t>
+  </si>
+  <si>
+    <t>//*[@id="datePickerMonthYearInput"]</t>
   </si>
 </sst>
 </file>
@@ -977,8 +1022,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A118">
-      <selection activeCell="A120" sqref="A120"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A136">
+      <selection activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
@@ -2358,16 +2403,104 @@
         <v>6</v>
       </c>
     </row>
-    <row r="135" ht="14.25" customHeight="1"/>
-    <row r="136" ht="14.25" customHeight="1"/>
-    <row r="137" ht="14.25" customHeight="1"/>
-    <row r="138" ht="14.25" customHeight="1"/>
-    <row r="139" ht="14.25" customHeight="1"/>
-    <row r="140" ht="14.25" customHeight="1"/>
-    <row r="141" ht="14.25" customHeight="1"/>
-    <row r="142" ht="14.25" customHeight="1"/>
-    <row r="143" ht="14.25" customHeight="1"/>
-    <row r="144" ht="14.25" customHeight="1"/>
+    <row r="135" ht="14.25" customHeight="1">
+      <c r="A135" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="136" ht="14.25" customHeight="1">
+      <c r="A136" t="s">
+        <v>233</v>
+      </c>
+      <c r="B136" t="s">
+        <v>173</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="137" ht="14.25" customHeight="1">
+      <c r="A137" t="s">
+        <v>234</v>
+      </c>
+      <c r="B137" t="s">
+        <v>235</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="138" ht="14.25" customHeight="1">
+      <c r="A138" t="s">
+        <v>236</v>
+      </c>
+      <c r="B138" t="s">
+        <v>237</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="139" ht="14.25" customHeight="1">
+      <c r="A139" t="s">
+        <v>234</v>
+      </c>
+      <c r="B139" t="s">
+        <v>238</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="140" ht="14.25" customHeight="1">
+      <c r="A140" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="141" ht="14.25" customHeight="1">
+      <c r="A141" t="s">
+        <v>240</v>
+      </c>
+      <c r="B141" t="s">
+        <v>186</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="142" ht="14.25" customHeight="1">
+      <c r="A142" t="s">
+        <v>241</v>
+      </c>
+      <c r="B142" t="s">
+        <v>242</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="143" ht="14.25" customHeight="1">
+      <c r="A143" t="s">
+        <v>243</v>
+      </c>
+      <c r="B143" t="s">
+        <v>244</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="144" ht="14.25" customHeight="1">
+      <c r="A144" t="s">
+        <v>245</v>
+      </c>
+      <c r="B144" t="s">
+        <v>246</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="145" ht="14.25" customHeight="1"/>
     <row r="146" ht="14.25" customHeight="1"/>
     <row r="147" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Widgets - Progress Bar
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -776,6 +776,24 @@
   </si>
   <si>
     <t>//*[@id="sliderContainer"]/div[2]</t>
+  </si>
+  <si>
+    <t>progressBar</t>
+  </si>
+  <si>
+    <t>progressBarNav</t>
+  </si>
+  <si>
+    <t>startProgressButton</t>
+  </si>
+  <si>
+    <t>//button[@id='startStopButton']</t>
+  </si>
+  <si>
+    <t>progressBarValue</t>
+  </si>
+  <si>
+    <t>//*[@id="progressBar"]/div</t>
   </si>
 </sst>
 </file>
@@ -1040,8 +1058,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A136">
-      <selection activeCell="B152" sqref="B152"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A145">
+      <selection activeCell="A155" sqref="A155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
@@ -2557,10 +2575,44 @@
         <v>6</v>
       </c>
     </row>
-    <row r="149" ht="14.25" customHeight="1"/>
-    <row r="150" ht="14.25" customHeight="1"/>
-    <row r="151" ht="14.25" customHeight="1"/>
-    <row r="152" ht="14.25" customHeight="1"/>
+    <row r="149" ht="14.25" customHeight="1">
+      <c r="A149" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="150" ht="14.25" customHeight="1">
+      <c r="A150" t="s">
+        <v>254</v>
+      </c>
+      <c r="B150" t="s">
+        <v>206</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="151" ht="14.25" customHeight="1">
+      <c r="A151" t="s">
+        <v>255</v>
+      </c>
+      <c r="B151" t="s">
+        <v>256</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="152" ht="14.25" customHeight="1">
+      <c r="A152" t="s">
+        <v>257</v>
+      </c>
+      <c r="B152" t="s">
+        <v>258</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="153" ht="14.25" customHeight="1"/>
     <row r="154" ht="14.25" customHeight="1"/>
     <row r="155" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Widgets - Tool Tips
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -824,6 +824,27 @@
   </si>
   <si>
     <t>//a[@id='demo-tab-use']</t>
+  </si>
+  <si>
+    <t>ToolTips</t>
+  </si>
+  <si>
+    <t>toolTipsNav</t>
+  </si>
+  <si>
+    <t>//div[@class='element-list collapse show']//li[@id='item-6']</t>
+  </si>
+  <si>
+    <t>BtnTooltipElement</t>
+  </si>
+  <si>
+    <t>//button[@id='toolTipButton']</t>
+  </si>
+  <si>
+    <t>tooltipText</t>
+  </si>
+  <si>
+    <t>//div[@class='tooltip-inner']</t>
   </si>
 </sst>
 </file>
@@ -1089,7 +1110,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A145">
-      <selection activeCell="B157" sqref="B157"/>
+      <selection activeCell="B162" sqref="B162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
@@ -2703,10 +2724,44 @@
         <v>6</v>
       </c>
     </row>
-    <row r="159" ht="14.25" customHeight="1"/>
-    <row r="160" ht="14.25" customHeight="1"/>
-    <row r="161" ht="14.25" customHeight="1"/>
-    <row r="162" ht="14.25" customHeight="1"/>
+    <row r="159" ht="14.25" customHeight="1">
+      <c r="A159" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="160" ht="14.25" customHeight="1">
+      <c r="A160" t="s">
+        <v>270</v>
+      </c>
+      <c r="B160" t="s">
+        <v>271</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="161" ht="14.25" customHeight="1">
+      <c r="A161" t="s">
+        <v>272</v>
+      </c>
+      <c r="B161" t="s">
+        <v>273</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="162" ht="14.25" customHeight="1">
+      <c r="A162" t="s">
+        <v>274</v>
+      </c>
+      <c r="B162" t="s">
+        <v>275</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="163" ht="14.25" customHeight="1"/>
     <row r="164" ht="14.25" customHeight="1"/>
     <row r="165" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Widgets - Select Menu
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -884,6 +884,51 @@
   </si>
   <si>
     <t>//h1[normalize-space()='Menu']</t>
+  </si>
+  <si>
+    <t>selectMenu</t>
+  </si>
+  <si>
+    <t>selectMenuNav</t>
+  </si>
+  <si>
+    <t>//div[@class='element-list collapse show']//li[@id='item-8']</t>
+  </si>
+  <si>
+    <t>selectMenuElement</t>
+  </si>
+  <si>
+    <t>//*[@id="withOptGroup"]/div/div[2]/div</t>
+  </si>
+  <si>
+    <t>selectedOptionElement</t>
+  </si>
+  <si>
+    <t>//*[@id="react-select-23-option-2"]</t>
+  </si>
+  <si>
+    <t>selectMenuScroll</t>
+  </si>
+  <si>
+    <t>//h1[normalize-space()='Select Menu']</t>
+  </si>
+  <si>
+    <t>selectOne</t>
+  </si>
+  <si>
+    <t>//*[@id="selectOne"]/div[1]/div[2]/div</t>
+  </si>
+  <si>
+    <t>OldStyleMenuSelect</t>
+  </si>
+  <si>
+    <t>//*[@id="oldSelectMenu"]</t>
+  </si>
+  <si>
+    <t>MultiMenuSelect</t>
+  </si>
+  <si>
+    <t>//*[@id="selectMenuContainer"]/div[7]/div/div/div</t>
   </si>
 </sst>
 </file>
@@ -1149,7 +1194,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A160">
-      <selection activeCell="B178" sqref="B178"/>
+      <selection activeCell="B176" sqref="B176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
@@ -2872,14 +2917,88 @@
         <v>6</v>
       </c>
     </row>
-    <row r="170" ht="14.25" customHeight="1"/>
-    <row r="171" ht="14.25" customHeight="1"/>
-    <row r="172" ht="14.25" customHeight="1"/>
-    <row r="173" ht="14.25" customHeight="1"/>
-    <row r="174" ht="14.25" customHeight="1"/>
-    <row r="175" ht="14.25" customHeight="1"/>
-    <row r="176" ht="14.25" customHeight="1"/>
-    <row r="177" ht="14.25" customHeight="1"/>
+    <row r="170" ht="14.25" customHeight="1">
+      <c r="A170" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="171" ht="14.25" customHeight="1">
+      <c r="A171" t="s">
+        <v>290</v>
+      </c>
+      <c r="B171" t="s">
+        <v>291</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="172" ht="14.25" customHeight="1">
+      <c r="A172" t="s">
+        <v>292</v>
+      </c>
+      <c r="B172" t="s">
+        <v>293</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="173" ht="14.25" customHeight="1">
+      <c r="A173" t="s">
+        <v>294</v>
+      </c>
+      <c r="B173" t="s">
+        <v>295</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="174" ht="14.25" customHeight="1">
+      <c r="A174" t="s">
+        <v>296</v>
+      </c>
+      <c r="B174" t="s">
+        <v>297</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="175" ht="14.25" customHeight="1">
+      <c r="A175" t="s">
+        <v>298</v>
+      </c>
+      <c r="B175" t="s">
+        <v>299</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="176" ht="14.25" customHeight="1">
+      <c r="A176" t="s">
+        <v>300</v>
+      </c>
+      <c r="B176" t="s">
+        <v>301</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="177" ht="14.25" customHeight="1">
+      <c r="A177" t="s">
+        <v>302</v>
+      </c>
+      <c r="B177" t="s">
+        <v>303</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="178" ht="14.25" customHeight="1"/>
     <row r="179" ht="14.25" customHeight="1"/>
     <row r="180" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Book Store Page - Login
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -58,6 +58,12 @@
     <t>//*[@id="app"]/div/div/div[2]/div/div[5]</t>
   </si>
   <si>
+    <t>bookStore</t>
+  </si>
+  <si>
+    <t>//div[@id='app']//div[6]</t>
+  </si>
+  <si>
     <t>forms</t>
   </si>
   <si>
@@ -1085,6 +1091,84 @@
   </si>
   <si>
     <t>draggedP4</t>
+  </si>
+  <si>
+    <t>Book Store</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>LoginNav</t>
+  </si>
+  <si>
+    <t>LoginScroll</t>
+  </si>
+  <si>
+    <t>//h1[normalize-space()='Login']</t>
+  </si>
+  <si>
+    <t>newUserBtn</t>
+  </si>
+  <si>
+    <t>//button[@id='newUser']</t>
+  </si>
+  <si>
+    <t>registerScroll</t>
+  </si>
+  <si>
+    <t>//h1[normalize-space()='Register']</t>
+  </si>
+  <si>
+    <t>registerFirstName</t>
+  </si>
+  <si>
+    <t>//*[@id="firstname"]</t>
+  </si>
+  <si>
+    <t>registerScndName</t>
+  </si>
+  <si>
+    <t>//*[@id="lastname"]</t>
+  </si>
+  <si>
+    <t>registerUserName</t>
+  </si>
+  <si>
+    <t>registerPassword</t>
+  </si>
+  <si>
+    <t>//*[@id="password"]</t>
+  </si>
+  <si>
+    <t>registerBtn</t>
+  </si>
+  <si>
+    <t>//*[@id="register"]</t>
+  </si>
+  <si>
+    <t>registerBckToLogin</t>
+  </si>
+  <si>
+    <t>//*[@id="gotologin"]</t>
+  </si>
+  <si>
+    <t>loginUserName</t>
+  </si>
+  <si>
+    <t>loginPassword</t>
+  </si>
+  <si>
+    <t>loginBtn</t>
+  </si>
+  <si>
+    <t>//*[@id="login"]</t>
+  </si>
+  <si>
+    <t>loggedusercheck</t>
+  </si>
+  <si>
+    <t>//*[@id="userName-value"]</t>
   </si>
 </sst>
 </file>
@@ -1349,8 +1433,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A193">
-      <selection activeCell="B196" sqref="B196"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A211">
+      <selection activeCell="B222" sqref="B222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
@@ -1424,44 +1508,44 @@
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" ht="22.5" customHeight="1">
-      <c r="A8" s="2" t="s">
+    <row r="8" ht="14.25" customHeight="1">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" ht="22.5" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1516,18 +1600,18 @@
       <c r="A16" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="C17" s="1"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" t="s">
@@ -1566,18 +1650,18 @@
       <c r="A21" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="1"/>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="C22" s="1"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="A23" t="s">
@@ -1602,21 +1686,21 @@
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="4" t="s">
+      <c r="A25" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="1"/>
+      <c r="B25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="C26" s="1"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="4" t="s">
@@ -1675,21 +1759,21 @@
     </row>
     <row r="32" ht="14.25" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" t="s">
-        <v>58</v>
+      <c r="A33" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>6</v>
@@ -1722,7 +1806,7 @@
         <v>64</v>
       </c>
       <c r="B36" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>6</v>
@@ -1730,10 +1814,10 @@
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>6</v>
@@ -1787,16 +1871,16 @@
       <c r="A42" t="s">
         <v>75</v>
       </c>
+      <c r="B42" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" t="s">
-        <v>76</v>
-      </c>
-      <c r="B43" t="s">
         <v>77</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -1880,16 +1964,16 @@
       <c r="A51" t="s">
         <v>92</v>
       </c>
+      <c r="B51" t="s">
+        <v>93</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" t="s">
-        <v>93</v>
-      </c>
-      <c r="B52" t="s">
         <v>94</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -1984,16 +2068,16 @@
       <c r="A61" t="s">
         <v>111</v>
       </c>
+      <c r="B61" t="s">
+        <v>112</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
       <c r="A62" t="s">
-        <v>112</v>
-      </c>
-      <c r="B62" t="s">
         <v>113</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="63" ht="14.25" customHeight="1">
@@ -2012,7 +2096,7 @@
         <v>116</v>
       </c>
       <c r="B64" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>6</v>
@@ -2020,18 +2104,18 @@
     </row>
     <row r="65" ht="14.25" customHeight="1">
       <c r="A65" t="s">
-        <v>117</v>
+        <v>118</v>
+      </c>
+      <c r="B65" t="s">
+        <v>81</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" t="s">
-        <v>118</v>
-      </c>
-      <c r="B66" t="s">
         <v>119</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
@@ -2039,7 +2123,7 @@
         <v>120</v>
       </c>
       <c r="B67" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>6</v>
@@ -2047,10 +2131,10 @@
     </row>
     <row r="68" ht="14.25" customHeight="1">
       <c r="A68" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B68" t="s">
-        <v>122</v>
+        <v>81</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>6</v>
@@ -2082,16 +2166,16 @@
       <c r="A71" t="s">
         <v>127</v>
       </c>
+      <c r="B71" t="s">
+        <v>128</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" t="s">
-        <v>128</v>
-      </c>
-      <c r="B72" t="s">
         <v>129</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
@@ -2099,7 +2183,7 @@
         <v>130</v>
       </c>
       <c r="B73" t="s">
-        <v>79</v>
+        <v>131</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>6</v>
@@ -2107,10 +2191,10 @@
     </row>
     <row r="74" ht="14.25" customHeight="1">
       <c r="A74" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B74" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>6</v>
@@ -2138,31 +2222,31 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="22.5" customHeight="1">
-      <c r="A78" s="2" t="s">
+    <row r="77" ht="14.25" customHeight="1">
+      <c r="A77" t="s">
         <v>137</v>
       </c>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
-    </row>
-    <row r="79" ht="14.25" customHeight="1">
-      <c r="A79" t="s">
+      <c r="B77" t="s">
         <v>138</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C77" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" ht="14.25" customHeight="1"/>
+    <row r="79" ht="22.5" customHeight="1">
+      <c r="A79" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
     </row>
     <row r="80" ht="14.25" customHeight="1">
       <c r="A80" t="s">
         <v>140</v>
       </c>
       <c r="B80" t="s">
-        <v>55</v>
+        <v>141</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>6</v>
@@ -2170,7 +2254,7 @@
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B81" t="s">
         <v>57</v>
@@ -2181,10 +2265,10 @@
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B82" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>6</v>
@@ -2192,10 +2276,10 @@
     </row>
     <row r="83" ht="14.25" customHeight="1">
       <c r="A83" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B83" t="s">
-        <v>144</v>
+        <v>24</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>6</v>
@@ -2272,7 +2356,7 @@
         <v>157</v>
       </c>
       <c r="B90" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>6</v>
@@ -2280,10 +2364,10 @@
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B91" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>6</v>
@@ -2291,10 +2375,10 @@
     </row>
     <row r="92" ht="14.25" customHeight="1">
       <c r="A92" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B92" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>6</v>
@@ -2302,38 +2386,38 @@
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B93" t="s">
-        <v>161</v>
+        <v>81</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="94" ht="22.5" customHeight="1">
-      <c r="A94" s="2" t="s">
+    <row r="94" ht="14.25" customHeight="1">
+      <c r="A94" t="s">
         <v>162</v>
       </c>
-      <c r="B94" s="3"/>
-      <c r="C94" s="3"/>
+      <c r="B94" t="s">
+        <v>163</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="95" ht="22.5" customHeight="1">
       <c r="A95" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B95" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="96" ht="14.25" customHeight="1">
-      <c r="A96" t="s">
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+    </row>
+    <row r="96" ht="22.5" customHeight="1">
+      <c r="A96" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C96" s="1" t="s">
@@ -2377,16 +2461,16 @@
       <c r="A100" t="s">
         <v>173</v>
       </c>
+      <c r="B100" t="s">
+        <v>174</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
       <c r="A101" t="s">
-        <v>174</v>
-      </c>
-      <c r="B101" t="s">
         <v>175</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="102" ht="14.25" customHeight="1">
@@ -2448,16 +2532,16 @@
       <c r="A107" t="s">
         <v>186</v>
       </c>
+      <c r="B107" t="s">
+        <v>187</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" t="s">
-        <v>187</v>
-      </c>
-      <c r="B108" t="s">
         <v>188</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
@@ -2498,7 +2582,7 @@
         <v>195</v>
       </c>
       <c r="B112" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>6</v>
@@ -2506,18 +2590,18 @@
     </row>
     <row r="113" ht="14.25" customHeight="1">
       <c r="A113" t="s">
-        <v>196</v>
+        <v>197</v>
+      </c>
+      <c r="B113" t="s">
+        <v>194</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" t="s">
-        <v>197</v>
-      </c>
-      <c r="B114" t="s">
         <v>198</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
@@ -2525,7 +2609,7 @@
         <v>199</v>
       </c>
       <c r="B115" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>6</v>
@@ -2533,10 +2617,10 @@
     </row>
     <row r="116" ht="14.25" customHeight="1">
       <c r="A116" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B116" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>6</v>
@@ -2568,16 +2652,16 @@
       <c r="A119" t="s">
         <v>206</v>
       </c>
+      <c r="B119" t="s">
+        <v>207</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="120" ht="14.25" customHeight="1">
       <c r="A120" t="s">
-        <v>207</v>
-      </c>
-      <c r="B120" t="s">
         <v>208</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="121" ht="14.25" customHeight="1">
@@ -2624,30 +2708,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="125" ht="22.5" customHeight="1">
-      <c r="A125" s="2" t="s">
+    <row r="125" ht="14.25" customHeight="1">
+      <c r="A125" t="s">
+        <v>217</v>
+      </c>
+      <c r="B125" t="s">
+        <v>218</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" ht="22.5" customHeight="1">
+      <c r="A126" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B125" s="3"/>
-      <c r="C125" s="3"/>
-    </row>
-    <row r="126" ht="14.25" customHeight="1">
-      <c r="A126" t="s">
-        <v>217</v>
-      </c>
-      <c r="B126" t="s">
-        <v>218</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B126" s="3"/>
+      <c r="C126" s="3"/>
     </row>
     <row r="127" ht="14.25" customHeight="1">
       <c r="A127" t="s">
         <v>219</v>
       </c>
       <c r="B127" t="s">
-        <v>166</v>
+        <v>220</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>6</v>
@@ -2655,10 +2739,10 @@
     </row>
     <row r="128" ht="14.25" customHeight="1">
       <c r="A128" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B128" t="s">
-        <v>221</v>
+        <v>168</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>6</v>
@@ -2713,7 +2797,7 @@
         <v>230</v>
       </c>
       <c r="B133" t="s">
-        <v>33</v>
+        <v>231</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>6</v>
@@ -2721,10 +2805,10 @@
     </row>
     <row r="134" ht="14.25" customHeight="1">
       <c r="A134" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B134" t="s">
-        <v>232</v>
+        <v>35</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>6</v>
@@ -2735,7 +2819,7 @@
         <v>233</v>
       </c>
       <c r="B135" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>6</v>
@@ -2743,26 +2827,26 @@
     </row>
     <row r="136" ht="14.25" customHeight="1">
       <c r="A136" t="s">
-        <v>234</v>
+        <v>235</v>
+      </c>
+      <c r="B136" t="s">
+        <v>220</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="137" ht="14.25" customHeight="1">
       <c r="A137" t="s">
-        <v>235</v>
-      </c>
-      <c r="B137" t="s">
-        <v>175</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>6</v>
+        <v>236</v>
       </c>
     </row>
     <row r="138" ht="14.25" customHeight="1">
       <c r="A138" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B138" t="s">
-        <v>237</v>
+        <v>177</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>6</v>
@@ -2781,10 +2865,10 @@
     </row>
     <row r="140" ht="14.25" customHeight="1">
       <c r="A140" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B140" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>6</v>
@@ -2792,26 +2876,26 @@
     </row>
     <row r="141" ht="14.25" customHeight="1">
       <c r="A141" t="s">
-        <v>241</v>
+        <v>238</v>
+      </c>
+      <c r="B141" t="s">
+        <v>242</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="142" ht="14.25" customHeight="1">
       <c r="A142" t="s">
-        <v>242</v>
-      </c>
-      <c r="B142" t="s">
-        <v>188</v>
-      </c>
-      <c r="C142" s="1" t="s">
-        <v>6</v>
+        <v>243</v>
       </c>
     </row>
     <row r="143" ht="14.25" customHeight="1">
       <c r="A143" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B143" t="s">
-        <v>244</v>
+        <v>190</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>6</v>
@@ -2843,24 +2927,24 @@
       <c r="A146" t="s">
         <v>249</v>
       </c>
+      <c r="B146" t="s">
+        <v>250</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="147" ht="14.25" customHeight="1">
       <c r="A147" t="s">
-        <v>250</v>
-      </c>
-      <c r="B147" t="s">
-        <v>198</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>6</v>
+        <v>251</v>
       </c>
     </row>
     <row r="148" ht="14.25" customHeight="1">
       <c r="A148" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B148" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>6</v>
@@ -2881,24 +2965,24 @@
       <c r="A150" t="s">
         <v>255</v>
       </c>
+      <c r="B150" t="s">
+        <v>256</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="151" ht="14.25" customHeight="1">
       <c r="A151" t="s">
-        <v>256</v>
-      </c>
-      <c r="B151" t="s">
-        <v>208</v>
-      </c>
-      <c r="C151" s="1" t="s">
-        <v>6</v>
+        <v>257</v>
       </c>
     </row>
     <row r="152" ht="14.25" customHeight="1">
       <c r="A152" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B152" t="s">
-        <v>258</v>
+        <v>210</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>6</v>
@@ -2919,16 +3003,16 @@
       <c r="A154" t="s">
         <v>261</v>
       </c>
+      <c r="B154" t="s">
+        <v>262</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="155" ht="14.25" customHeight="1">
       <c r="A155" t="s">
-        <v>262</v>
-      </c>
-      <c r="B155" t="s">
         <v>263</v>
-      </c>
-      <c r="C155" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="156" ht="14.25" customHeight="1">
@@ -2947,7 +3031,7 @@
         <v>266</v>
       </c>
       <c r="B157" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>6</v>
@@ -2955,10 +3039,10 @@
     </row>
     <row r="158" ht="14.25" customHeight="1">
       <c r="A158" t="s">
+        <v>268</v>
+      </c>
+      <c r="B158" t="s">
         <v>267</v>
-      </c>
-      <c r="B158" t="s">
-        <v>268</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>6</v>
@@ -2979,16 +3063,16 @@
       <c r="A160" t="s">
         <v>271</v>
       </c>
+      <c r="B160" t="s">
+        <v>272</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="161" ht="14.25" customHeight="1">
       <c r="A161" t="s">
-        <v>272</v>
-      </c>
-      <c r="B161" t="s">
         <v>273</v>
-      </c>
-      <c r="C161" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="162" ht="14.25" customHeight="1">
@@ -3017,16 +3101,16 @@
       <c r="A164" t="s">
         <v>278</v>
       </c>
+      <c r="B164" t="s">
+        <v>279</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="165" ht="14.25" customHeight="1">
       <c r="A165" t="s">
-        <v>279</v>
-      </c>
-      <c r="B165" t="s">
         <v>280</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="166" ht="14.25" customHeight="1">
@@ -3088,16 +3172,16 @@
       <c r="A171" t="s">
         <v>291</v>
       </c>
+      <c r="B171" t="s">
+        <v>292</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="172" ht="14.25" customHeight="1">
       <c r="A172" t="s">
-        <v>292</v>
-      </c>
-      <c r="B172" t="s">
         <v>293</v>
-      </c>
-      <c r="C172" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="173" ht="14.25" customHeight="1">
@@ -3166,35 +3250,35 @@
         <v>6</v>
       </c>
     </row>
-    <row r="179" ht="22.5" customHeight="1">
-      <c r="A179" s="2" t="s">
+    <row r="179" ht="14.25" customHeight="1">
+      <c r="A179" t="s">
         <v>306</v>
       </c>
-      <c r="B179" s="3"/>
-      <c r="C179" s="3"/>
-    </row>
-    <row r="180" ht="14.25" customHeight="1">
-      <c r="A180" t="s">
+      <c r="B179" t="s">
         <v>307</v>
       </c>
+      <c r="C179" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="180" ht="22.5" customHeight="1">
+      <c r="A180" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B180" s="3"/>
+      <c r="C180" s="3"/>
     </row>
     <row r="181" ht="14.25" customHeight="1">
       <c r="A181" t="s">
-        <v>308</v>
-      </c>
-      <c r="B181" t="s">
-        <v>166</v>
-      </c>
-      <c r="C181" s="1" t="s">
-        <v>6</v>
+        <v>309</v>
       </c>
     </row>
     <row r="182" ht="14.25" customHeight="1">
       <c r="A182" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B182" t="s">
-        <v>310</v>
+        <v>168</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>6</v>
@@ -3248,24 +3332,24 @@
       <c r="A187" t="s">
         <v>319</v>
       </c>
+      <c r="B187" t="s">
+        <v>320</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="188" ht="14.25" customHeight="1">
       <c r="A188" t="s">
-        <v>320</v>
-      </c>
-      <c r="B188" t="s">
-        <v>175</v>
-      </c>
-      <c r="C188" s="1" t="s">
-        <v>6</v>
+        <v>321</v>
       </c>
     </row>
     <row r="189" ht="14.25" customHeight="1">
       <c r="A189" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B189" t="s">
-        <v>322</v>
+        <v>177</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>6</v>
@@ -3287,7 +3371,7 @@
         <v>325</v>
       </c>
       <c r="B191" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>6</v>
@@ -3295,10 +3379,10 @@
     </row>
     <row r="192" ht="14.25" customHeight="1">
       <c r="A192" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B192" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>6</v>
@@ -3341,24 +3425,24 @@
       <c r="A196" t="s">
         <v>334</v>
       </c>
+      <c r="B196" t="s">
+        <v>335</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="197" ht="14.25" customHeight="1">
       <c r="A197" t="s">
-        <v>335</v>
-      </c>
-      <c r="B197" t="s">
-        <v>188</v>
-      </c>
-      <c r="C197" s="1" t="s">
-        <v>6</v>
+        <v>336</v>
       </c>
     </row>
     <row r="198" ht="14.25" customHeight="1">
       <c r="A198" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B198" t="s">
-        <v>337</v>
+        <v>190</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>6</v>
@@ -3379,25 +3463,25 @@
       <c r="A200" t="s">
         <v>340</v>
       </c>
-      <c r="C200" s="1"/>
+      <c r="B200" t="s">
+        <v>341</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="201" ht="14.25" customHeight="1">
       <c r="A201" t="s">
-        <v>341</v>
-      </c>
-      <c r="B201" t="s">
-        <v>198</v>
-      </c>
-      <c r="C201" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>342</v>
+      </c>
+      <c r="C201" s="1"/>
     </row>
     <row r="202" ht="14.25" customHeight="1">
       <c r="A202" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B202" t="s">
-        <v>343</v>
+        <v>200</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>6</v>
@@ -3418,24 +3502,24 @@
       <c r="A204" t="s">
         <v>346</v>
       </c>
+      <c r="B204" t="s">
+        <v>347</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="205" ht="14.25" customHeight="1">
       <c r="A205" t="s">
-        <v>347</v>
-      </c>
-      <c r="B205" t="s">
-        <v>208</v>
-      </c>
-      <c r="C205" s="1" t="s">
-        <v>6</v>
+        <v>348</v>
       </c>
     </row>
     <row r="206" ht="14.25" customHeight="1">
       <c r="A206" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B206" t="s">
-        <v>349</v>
+        <v>210</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>6</v>
@@ -3468,7 +3552,7 @@
         <v>354</v>
       </c>
       <c r="B209" t="s">
-        <v>79</v>
+        <v>355</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>6</v>
@@ -3476,29 +3560,191 @@
     </row>
     <row r="210" ht="14.25" customHeight="1">
       <c r="A210" t="s">
-        <v>355</v>
+        <v>356</v>
+      </c>
+      <c r="B210" t="s">
+        <v>81</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="211" ht="14.25" customHeight="1"/>
-    <row r="212" ht="14.25" customHeight="1"/>
-    <row r="213" ht="14.25" customHeight="1"/>
-    <row r="214" ht="14.25" customHeight="1"/>
-    <row r="215" ht="14.25" customHeight="1"/>
-    <row r="216" ht="14.25" customHeight="1"/>
-    <row r="217" ht="14.25" customHeight="1"/>
-    <row r="218" ht="14.25" customHeight="1"/>
-    <row r="219" ht="14.25" customHeight="1"/>
-    <row r="220" ht="14.25" customHeight="1"/>
-    <row r="221" ht="14.25" customHeight="1"/>
-    <row r="222" ht="14.25" customHeight="1"/>
-    <row r="223" ht="14.25" customHeight="1"/>
-    <row r="224" ht="14.25" customHeight="1"/>
-    <row r="225" ht="14.25" customHeight="1"/>
-    <row r="226" ht="14.25" customHeight="1"/>
-    <row r="227" ht="14.25" customHeight="1"/>
+    <row r="211" ht="14.25" customHeight="1">
+      <c r="A211" t="s">
+        <v>357</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="212" ht="22.5" customHeight="1">
+      <c r="A212" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B212" s="3"/>
+      <c r="C212" s="3"/>
+    </row>
+    <row r="213" ht="22.5" customHeight="1">
+      <c r="A213" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B213" s="3"/>
+      <c r="C213" s="3"/>
+    </row>
+    <row r="214" ht="14.25" customHeight="1">
+      <c r="A214" t="s">
+        <v>360</v>
+      </c>
+      <c r="B214" t="s">
+        <v>168</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="215" ht="14.25" customHeight="1">
+      <c r="A215" t="s">
+        <v>361</v>
+      </c>
+      <c r="B215" t="s">
+        <v>362</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="216" ht="14.25" customHeight="1">
+      <c r="A216" t="s">
+        <v>363</v>
+      </c>
+      <c r="B216" t="s">
+        <v>364</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="217" ht="14.25" customHeight="1">
+      <c r="A217" t="s">
+        <v>365</v>
+      </c>
+      <c r="B217" t="s">
+        <v>366</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="218" ht="14.25" customHeight="1">
+      <c r="A218" t="s">
+        <v>367</v>
+      </c>
+      <c r="B218" t="s">
+        <v>368</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="219" ht="14.25" customHeight="1">
+      <c r="A219" t="s">
+        <v>369</v>
+      </c>
+      <c r="B219" t="s">
+        <v>370</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="220" ht="14.25" customHeight="1">
+      <c r="A220" t="s">
+        <v>371</v>
+      </c>
+      <c r="B220" t="s">
+        <v>22</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="221" ht="14.25" customHeight="1">
+      <c r="A221" t="s">
+        <v>372</v>
+      </c>
+      <c r="B221" t="s">
+        <v>373</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="222" ht="14.25" customHeight="1">
+      <c r="A222" t="s">
+        <v>374</v>
+      </c>
+      <c r="B222" t="s">
+        <v>375</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="223" ht="14.25" customHeight="1">
+      <c r="A223" t="s">
+        <v>376</v>
+      </c>
+      <c r="B223" t="s">
+        <v>377</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="224" ht="14.25" customHeight="1">
+      <c r="A224" t="s">
+        <v>378</v>
+      </c>
+      <c r="B224" t="s">
+        <v>22</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="225" ht="14.25" customHeight="1">
+      <c r="A225" t="s">
+        <v>379</v>
+      </c>
+      <c r="B225" t="s">
+        <v>373</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="226" ht="14.25" customHeight="1">
+      <c r="A226" t="s">
+        <v>380</v>
+      </c>
+      <c r="B226" t="s">
+        <v>381</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="227" ht="14.25" customHeight="1">
+      <c r="A227" t="s">
+        <v>382</v>
+      </c>
+      <c r="B227" t="s">
+        <v>383</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="228" ht="14.25" customHeight="1"/>
     <row r="229" ht="14.25" customHeight="1"/>
     <row r="230" ht="14.25" customHeight="1"/>
@@ -4266,14 +4512,17 @@
     <row r="992" ht="14.25" customHeight="1"/>
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
+    <row r="995" ht="14.25" customHeight="1"/>
+    <row r="996" ht="14.25" customHeight="1"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A94:C94"/>
-    <mergeCell ref="A125:C125"/>
-    <mergeCell ref="A179:C179"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A79:C79"/>
+    <mergeCell ref="A95:C95"/>
+    <mergeCell ref="A126:C126"/>
+    <mergeCell ref="A180:C180"/>
+    <mergeCell ref="A212:C212"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Book Store Page - Books Search & select
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -1169,6 +1169,21 @@
   </si>
   <si>
     <t>//*[@id="userName-value"]</t>
+  </si>
+  <si>
+    <t>BookStore</t>
+  </si>
+  <si>
+    <t>bookStoreSearch</t>
+  </si>
+  <si>
+    <t>//input[@id='searchBox']</t>
+  </si>
+  <si>
+    <t>selectBook</t>
+  </si>
+  <si>
+    <t>//*[@id="see-book-Eloquent JavaScript, Second Edition"]/a</t>
   </si>
 </sst>
 </file>
@@ -1433,8 +1448,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A211">
-      <selection activeCell="B222" sqref="B222"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" topLeftCell="A223">
+      <selection activeCell="A232" sqref="A232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
@@ -3745,9 +3760,33 @@
         <v>6</v>
       </c>
     </row>
-    <row r="228" ht="14.25" customHeight="1"/>
-    <row r="229" ht="14.25" customHeight="1"/>
-    <row r="230" ht="14.25" customHeight="1"/>
+    <row r="228" ht="14.25" customHeight="1">
+      <c r="A228" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="229" ht="14.25" customHeight="1">
+      <c r="A229" t="s">
+        <v>385</v>
+      </c>
+      <c r="B229" t="s">
+        <v>386</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="230" ht="14.25" customHeight="1">
+      <c r="A230" t="s">
+        <v>387</v>
+      </c>
+      <c r="B230" t="s">
+        <v>388</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="231" ht="14.25" customHeight="1"/>
     <row r="232" ht="14.25" customHeight="1"/>
     <row r="233" ht="14.25" customHeight="1"/>

</xml_diff>